<commit_message>
Add new experimental results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA05FF72-482D-2E40-838E-B68CB329ECE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4CE9A7-F2FF-D94B-8A88-820A58013F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45880" yWindow="0" windowWidth="22920" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
+    <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Instanz</t>
   </si>
@@ -67,9 +67,6 @@
     <t>373,7…</t>
   </si>
   <si>
-    <t>E-n23k3</t>
-  </si>
-  <si>
     <t>493,0…</t>
   </si>
   <si>
@@ -134,6 +131,33 @@
   </si>
   <si>
     <t>670s</t>
+  </si>
+  <si>
+    <t>ng-Paths</t>
+  </si>
+  <si>
+    <t>E-n23-k3</t>
+  </si>
+  <si>
+    <t>558,6…</t>
+  </si>
+  <si>
+    <t>373,5…</t>
+  </si>
+  <si>
+    <t>190s</t>
+  </si>
+  <si>
+    <t>481,0…</t>
+  </si>
+  <si>
+    <t>292s</t>
+  </si>
+  <si>
+    <t>1002,2…</t>
+  </si>
+  <si>
+    <t>324s</t>
   </si>
 </sst>
 </file>
@@ -502,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,7 +538,7 @@
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,8 +557,14 @@
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -554,26 +584,35 @@
         <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>569</v>
       </c>
       <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>13</v>
       </c>
       <c r="B4">
         <v>547</v>
@@ -582,41 +621,47 @@
         <v>47</v>
       </c>
       <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>18</v>
       </c>
       <c r="B5">
         <v>835</v>
       </c>
       <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>22</v>
       </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>24</v>
       </c>
       <c r="B6">
         <v>521</v>
@@ -625,36 +670,42 @@
         <v>42</v>
       </c>
       <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>26</v>
       </c>
-      <c r="G6" t="s">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>28</v>
       </c>
       <c r="B7">
         <v>1021</v>
       </c>
       <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>31</v>
       </c>
-      <c r="G7" t="s">
-        <v>32</v>
+      <c r="K7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plot the results of the bounds at the same time
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4CE9A7-F2FF-D94B-8A88-820A58013F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A04A82-226B-B54C-A452-AD79E2E30268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Instanz</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>324s</t>
+  </si>
+  <si>
+    <t>Beobachtung</t>
+  </si>
+  <si>
+    <t>Nur eine verwendete Variable ist nicht elementar. DSSR sinnvoll für ESPPRC Lösung?</t>
   </si>
 </sst>
 </file>
@@ -526,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,7 +544,7 @@
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,8 +569,14 @@
       <c r="K1" s="1">
         <v>8</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -589,8 +601,11 @@
       <c r="K2" t="s">
         <v>35</v>
       </c>
+      <c r="N2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -610,7 +625,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -639,7 +654,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -659,7 +674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -682,7 +697,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -706,6 +721,9 @@
       </c>
       <c r="L7" t="s">
         <v>40</v>
+      </c>
+      <c r="M7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add heuristic method for finding initial variables
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A04A82-226B-B54C-A452-AD79E2E30268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ECA846-DC9C-AF45-A196-5DA071D8A4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22920" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Instanz</t>
   </si>
@@ -164,6 +164,27 @@
   </si>
   <si>
     <t>Nur eine verwendete Variable ist nicht elementar. DSSR sinnvoll für ESPPRC Lösung?</t>
+  </si>
+  <si>
+    <t>E-n101-k14</t>
+  </si>
+  <si>
+    <t>1023,2…</t>
+  </si>
+  <si>
+    <t>278s</t>
+  </si>
+  <si>
+    <t>X-n101-k25</t>
+  </si>
+  <si>
+    <t>26787,8…</t>
+  </si>
+  <si>
+    <t>97s</t>
+  </si>
+  <si>
+    <t>X-n129-k18</t>
   </si>
 </sst>
 </file>
@@ -532,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,6 +747,51 @@
         <v>42</v>
       </c>
     </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>1071</v>
+      </c>
+      <c r="C8">
+        <v>114</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10">
+        <v>27591</v>
+      </c>
+      <c r="C10">
+        <v>140</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>28940</v>
+      </c>
+      <c r="C11">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add time limit to pricer
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ECA846-DC9C-AF45-A196-5DA071D8A4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07B33AE-5756-1F4A-AF2D-DC25CB646F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22920" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
+    <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>Instanz</t>
   </si>
@@ -55,9 +55,6 @@
     <t>ESPPRC</t>
   </si>
   <si>
-    <t> E-n22-k4</t>
-  </si>
-  <si>
     <t>343,9…</t>
   </si>
   <si>
@@ -185,6 +182,30 @@
   </si>
   <si>
     <t>X-n129-k18</t>
+  </si>
+  <si>
+    <t>X-n106-k14</t>
+  </si>
+  <si>
+    <t>25186,2…</t>
+  </si>
+  <si>
+    <t>139s</t>
+  </si>
+  <si>
+    <t>E-n22-k4</t>
+  </si>
+  <si>
+    <t>558,9…</t>
+  </si>
+  <si>
+    <t>102s</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>time_limit=10, heuristic=10</t>
   </si>
 </sst>
 </file>
@@ -553,19 +574,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,21 +607,24 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="1">
+        <v>55</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="1">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="1">
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B2">
         <v>375</v>
@@ -608,96 +633,105 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
       <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>569</v>
       </c>
       <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
       <c r="B4">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="C4">
         <v>47</v>
       </c>
       <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>17</v>
       </c>
       <c r="B5">
         <v>835</v>
       </c>
       <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>23</v>
       </c>
       <c r="B6">
         <v>521</v>
@@ -706,50 +740,50 @@
         <v>42</v>
       </c>
       <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>27</v>
       </c>
       <c r="B7">
         <v>1021</v>
       </c>
       <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>30</v>
       </c>
-      <c r="G7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" t="s">
         <v>39</v>
       </c>
-      <c r="L7" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>43</v>
       </c>
       <c r="B8">
         <v>1071</v>
@@ -758,15 +792,15 @@
         <v>114</v>
       </c>
       <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>46</v>
       </c>
       <c r="B10">
         <v>27591</v>
@@ -775,20 +809,37 @@
         <v>140</v>
       </c>
       <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
         <v>47</v>
       </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>49</v>
       </c>
       <c r="B11">
+        <v>26362</v>
+      </c>
+      <c r="C11">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12">
         <v>28940</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Find an error in a large instance
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07B33AE-5756-1F4A-AF2D-DC25CB646F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB52539-B189-9E41-9D6A-90A2B82DF17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>Instanz</t>
   </si>
@@ -187,12 +187,6 @@
     <t>X-n106-k14</t>
   </si>
   <si>
-    <t>25186,2…</t>
-  </si>
-  <si>
-    <t>139s</t>
-  </si>
-  <si>
     <t>E-n22-k4</t>
   </si>
   <si>
@@ -206,6 +200,45 @@
   </si>
   <si>
     <t>time_limit=10, heuristic=10</t>
+  </si>
+  <si>
+    <t>time_limit 100 exceeded without paths</t>
+  </si>
+  <si>
+    <t>time_limit=100 exceeded</t>
+  </si>
+  <si>
+    <t>X-n110-k13</t>
+  </si>
+  <si>
+    <t>13924,6…</t>
+  </si>
+  <si>
+    <t>X-n115-k10</t>
+  </si>
+  <si>
+    <t>X-n120-k6</t>
+  </si>
+  <si>
+    <t>X-n125-k30</t>
+  </si>
+  <si>
+    <t>X-n256-k16</t>
+  </si>
+  <si>
+    <t>11982,7…</t>
+  </si>
+  <si>
+    <t>12308,0...</t>
+  </si>
+  <si>
+    <t>25186,2...</t>
+  </si>
+  <si>
+    <t>54998,2…</t>
+  </si>
+  <si>
+    <t>27830,8…</t>
   </si>
 </sst>
 </file>
@@ -574,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>31</v>
@@ -624,7 +657,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2">
         <v>375</v>
@@ -665,13 +698,13 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
         <v>54</v>
-      </c>
-      <c r="J3" t="s">
-        <v>56</v>
       </c>
       <c r="L3" t="s">
         <v>33</v>
@@ -702,6 +735,9 @@
       <c r="G4" t="s">
         <v>14</v>
       </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
       <c r="L4" t="s">
         <v>36</v>
       </c>
@@ -716,6 +752,9 @@
       <c r="B5">
         <v>835</v>
       </c>
+      <c r="C5">
+        <v>136</v>
+      </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
@@ -727,6 +766,9 @@
       </c>
       <c r="G5" t="s">
         <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -771,6 +813,9 @@
       <c r="G7" t="s">
         <v>30</v>
       </c>
+      <c r="J7" t="s">
+        <v>56</v>
+      </c>
       <c r="L7" t="s">
         <v>38</v>
       </c>
@@ -826,21 +871,82 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12">
+        <v>14971</v>
+      </c>
+      <c r="C12">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13">
+        <v>12747</v>
+      </c>
+      <c r="C13">
+        <v>171</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>13332</v>
+      </c>
+      <c r="C14">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15">
+        <v>55539</v>
+      </c>
+      <c r="C15">
+        <v>128</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>48</v>
       </c>
-      <c r="B12">
+      <c r="B16">
         <v>28940</v>
       </c>
-      <c r="C12">
+      <c r="C16">
         <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove usage of ctypes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB52539-B189-9E41-9D6A-90A2B82DF17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFA4667-8ED2-1546-8D5F-499ABE7DE509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>Instanz</t>
   </si>
@@ -239,6 +239,18 @@
   </si>
   <si>
     <t>27830,8…</t>
+  </si>
+  <si>
+    <t>X-n251-k28</t>
+  </si>
+  <si>
+    <t>X-n200-k36</t>
+  </si>
+  <si>
+    <t>57666,2…</t>
+  </si>
+  <si>
+    <t>X-n228-k23</t>
   </si>
 </sst>
 </file>
@@ -607,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,9 +956,48 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17">
+        <v>58578</v>
+      </c>
+      <c r="C17">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18">
+        <v>25742</v>
+      </c>
+      <c r="C18">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19">
+        <v>38684</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>62</v>
+      </c>
+      <c r="C20">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add first result for X-n502-k39
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFA4667-8ED2-1546-8D5F-499ABE7DE509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5C83E4-F454-C04D-84FC-4F2BE3376390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
   <si>
     <t>Instanz</t>
   </si>
@@ -251,6 +251,30 @@
   </si>
   <si>
     <t>X-n228-k23</t>
+  </si>
+  <si>
+    <t>36917,9…</t>
+  </si>
+  <si>
+    <t>X-n289-k60</t>
+  </si>
+  <si>
+    <t>69226(BKS)</t>
+  </si>
+  <si>
+    <t>18839(BKS)</t>
+  </si>
+  <si>
+    <t>67560,2…</t>
+  </si>
+  <si>
+    <t>262s mit Startheuristik</t>
+  </si>
+  <si>
+    <t>X-n502-k39</t>
+  </si>
+  <si>
+    <t>68165,5… (evt. Mit SPPRC Pfaden)</t>
   </si>
 </sst>
 </file>
@@ -619,16 +643,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -956,7 +981,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -970,7 +995,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -981,7 +1006,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -991,13 +1016,50 @@
       <c r="C19">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>62</v>
       </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
       <c r="C20">
         <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21">
+        <v>95151</v>
+      </c>
+      <c r="C21">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Export first result to latex
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5C83E4-F454-C04D-84FC-4F2BE3376390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55593098-6095-5B46-8D44-342EA4D1749F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -646,7 +646,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Not working version fo 2 cycle
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3769DBFF-E4F7-A747-BDB3-7BA2605760B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3023FB-024B-CE46-BEB7-860ECDB53009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
   <si>
     <t>Instanz</t>
   </si>
@@ -118,9 +118,6 @@
     <t>E-n76-k14</t>
   </si>
   <si>
-    <t>52 (aber eher um die 7)</t>
-  </si>
-  <si>
     <t>974,5…</t>
   </si>
   <si>
@@ -142,15 +139,9 @@
     <t>481,0…</t>
   </si>
   <si>
-    <t>292s</t>
-  </si>
-  <si>
     <t>1002,2…</t>
   </si>
   <si>
-    <t>324s</t>
-  </si>
-  <si>
     <t>Beobachtung</t>
   </si>
   <si>
@@ -163,18 +154,12 @@
     <t>1023,2…</t>
   </si>
   <si>
-    <t>278s</t>
-  </si>
-  <si>
     <t>X-n101-k25</t>
   </si>
   <si>
     <t>26787,8…</t>
   </si>
   <si>
-    <t>97s</t>
-  </si>
-  <si>
     <t>X-n129-k18</t>
   </si>
   <si>
@@ -256,9 +241,6 @@
     <t>67560,2…</t>
   </si>
   <si>
-    <t>262s mit Startheuristik</t>
-  </si>
-  <si>
     <t>X-n502-k39</t>
   </si>
   <si>
@@ -271,10 +253,64 @@
     <t>time_limit=300, heuristic=1 exceeded</t>
   </si>
   <si>
-    <t>119s</t>
-  </si>
-  <si>
     <t>time_limit=10</t>
+  </si>
+  <si>
+    <t>u … update am 22-06-07, h … mit Heuristik</t>
+  </si>
+  <si>
+    <t>22s (u)</t>
+  </si>
+  <si>
+    <t>32s (uh)</t>
+  </si>
+  <si>
+    <t>52 (realistisch 7)</t>
+  </si>
+  <si>
+    <t>282s (uh)</t>
+  </si>
+  <si>
+    <t>11s (uh)</t>
+  </si>
+  <si>
+    <t>2725,0…</t>
+  </si>
+  <si>
+    <t>80s (uh)</t>
+  </si>
+  <si>
+    <t>(uh) time_limit 300 exceeded</t>
+  </si>
+  <si>
+    <t>1s(uh)</t>
+  </si>
+  <si>
+    <t>114s (uh)</t>
+  </si>
+  <si>
+    <t>246s (uh)</t>
+  </si>
+  <si>
+    <t>time_limi=30</t>
+  </si>
+  <si>
+    <t>time_limit=60 exceeded</t>
+  </si>
+  <si>
+    <t>90s (uh)</t>
+  </si>
+  <si>
+    <t>16s (uh)</t>
+  </si>
+  <si>
+    <t>60s (uh)</t>
+  </si>
+  <si>
+    <t>14704,8…</t>
+  </si>
+  <si>
+    <t>210s (uh)</t>
   </si>
 </sst>
 </file>
@@ -304,7 +340,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -321,14 +357,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -645,16 +726,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="4"/>
+    <col min="5" max="5" width="36.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="4"/>
+    <col min="9" max="9" width="10.83203125" style="5"/>
+    <col min="10" max="10" width="24.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -667,26 +754,30 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>51</v>
+      <c r="J1" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L1" s="1">
         <v>8</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="O1" s="1">
         <v>20</v>
@@ -694,7 +785,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>375</v>
@@ -702,28 +793,31 @@
       <c r="C2">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="L2">
         <v>373.5</v>
       </c>
+      <c r="M2" t="s">
+        <v>82</v>
+      </c>
       <c r="O2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>569</v>
@@ -731,29 +825,29 @@
       <c r="C3">
         <v>69</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J3" t="s">
-        <v>77</v>
+      <c r="H3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -766,26 +860,29 @@
       <c r="C4">
         <v>47</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J4" t="s">
-        <v>76</v>
+      <c r="H4" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M4" t="s">
-        <v>35</v>
+        <v>84</v>
+      </c>
+      <c r="N4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -798,20 +895,23 @@
       <c r="C5">
         <v>136</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J5" t="s">
-        <v>52</v>
+      <c r="H5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -824,17 +924,21 @@
       <c r="C6">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="7" t="s">
         <v>25</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="L6" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -845,50 +949,56 @@
         <v>1021</v>
       </c>
       <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" t="s">
-        <v>52</v>
+      <c r="H7" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" t="s">
         <v>36</v>
-      </c>
-      <c r="M7" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="C8">
         <v>114</v>
       </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
+      <c r="D8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>27591</v>
@@ -896,16 +1006,22 @@
       <c r="C10">
         <v>140</v>
       </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
+      <c r="D10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" t="s">
+        <v>79</v>
+      </c>
+      <c r="M10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B11">
         <v>26362</v>
@@ -913,13 +1029,16 @@
       <c r="C11">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
-        <v>61</v>
+      <c r="D11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B12">
         <v>14971</v>
@@ -927,13 +1046,22 @@
       <c r="C12">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
-        <v>54</v>
+      <c r="D12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="L12" t="s">
+        <v>90</v>
+      </c>
+      <c r="M12" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B13">
         <v>12747</v>
@@ -941,13 +1069,13 @@
       <c r="C13">
         <v>171</v>
       </c>
-      <c r="D13" t="s">
-        <v>59</v>
+      <c r="D13" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B14">
         <v>13332</v>
@@ -955,13 +1083,13 @@
       <c r="C14">
         <v>23</v>
       </c>
-      <c r="D14" t="s">
-        <v>60</v>
+      <c r="D14" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B15">
         <v>55539</v>
@@ -969,13 +1097,13 @@
       <c r="C15">
         <v>128</v>
       </c>
-      <c r="D15" t="s">
-        <v>62</v>
+      <c r="D15" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>28940</v>
@@ -983,13 +1111,13 @@
       <c r="C16">
         <v>41</v>
       </c>
-      <c r="D16" t="s">
-        <v>63</v>
+      <c r="D16" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B17">
         <v>58578</v>
@@ -997,13 +1125,13 @@
       <c r="C17">
         <v>83</v>
       </c>
-      <c r="D17" t="s">
-        <v>66</v>
+      <c r="D17" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B18">
         <v>25742</v>
@@ -1014,7 +1142,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B19">
         <v>38684</v>
@@ -1022,16 +1150,16 @@
       <c r="C19">
         <v>16</v>
       </c>
-      <c r="D19" t="s">
-        <v>68</v>
+      <c r="D19" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C20">
         <v>27</v>
@@ -1039,7 +1167,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B21">
         <v>95151</v>
@@ -1050,22 +1178,22 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C22">
         <v>15</v>
       </c>
-      <c r="D22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" t="s">
-        <v>75</v>
+      <c r="D22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try to fix weird 2 cycle behavior, but that doesnt work out
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220A82A0-D8BF-C141-AAB1-491C902FB314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51CB3A0-C603-4E4C-AF9F-8907E2F1E9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="107">
   <si>
     <t>Instanz</t>
   </si>
@@ -64,30 +64,18 @@
     <t>493,0…</t>
   </si>
   <si>
-    <t>539,8…</t>
-  </si>
-  <si>
     <t>E-n30-k3</t>
   </si>
   <si>
     <t>445,0…</t>
   </si>
   <si>
-    <t>464,3…</t>
-  </si>
-  <si>
-    <t>40s</t>
-  </si>
-  <si>
     <t>11s</t>
   </si>
   <si>
     <t>E-n33-k4</t>
   </si>
   <si>
-    <t>10s</t>
-  </si>
-  <si>
     <t>776,6…</t>
   </si>
   <si>
@@ -97,21 +85,12 @@
     <t>793,1…</t>
   </si>
   <si>
-    <t>37s</t>
-  </si>
-  <si>
     <t>E-n51-k5</t>
   </si>
   <si>
     <t>494,5…</t>
   </si>
   <si>
-    <t>512,7…</t>
-  </si>
-  <si>
-    <t>80s</t>
-  </si>
-  <si>
     <t>E-n76-k14</t>
   </si>
   <si>
@@ -121,9 +100,6 @@
     <t>999,5…</t>
   </si>
   <si>
-    <t>670s</t>
-  </si>
-  <si>
     <t>ng-Paths</t>
   </si>
   <si>
@@ -238,115 +214,148 @@
     <t>X-n502-k39</t>
   </si>
   <si>
-    <t>68165,5… (evt. Mit SPPRC Pfaden)</t>
-  </si>
-  <si>
     <t>time_limit=10</t>
   </si>
   <si>
-    <t>u … update am 22-06-07, h … mit Heuristik</t>
-  </si>
-  <si>
-    <t>22s (u)</t>
-  </si>
-  <si>
-    <t>32s (uh)</t>
-  </si>
-  <si>
     <t>52 (realistisch 7)</t>
   </si>
   <si>
-    <t>282s (uh)</t>
-  </si>
-  <si>
-    <t>11s (uh)</t>
-  </si>
-  <si>
-    <t>2725,0…</t>
-  </si>
-  <si>
-    <t>80s (uh)</t>
-  </si>
-  <si>
     <t>(uh) time_limit 300 exceeded</t>
   </si>
   <si>
-    <t>1s(uh)</t>
-  </si>
-  <si>
-    <t>114s (uh)</t>
-  </si>
-  <si>
-    <t>246s (uh)</t>
-  </si>
-  <si>
     <t>time_limi=30</t>
   </si>
   <si>
     <t>time_limit=60 exceeded</t>
   </si>
   <si>
-    <t>90s (uh)</t>
-  </si>
-  <si>
-    <t>16s (uh)</t>
-  </si>
-  <si>
-    <t>60s (uh)</t>
-  </si>
-  <si>
     <t>14704,8…</t>
   </si>
   <si>
-    <t>210s (uh)</t>
-  </si>
-  <si>
-    <t>48s (uh)</t>
-  </si>
-  <si>
     <t xml:space="preserve">time_limit 600 exceeded </t>
   </si>
   <si>
     <t>(uh) time_limit 1200 exceeded (gesamt 3800s)</t>
   </si>
   <si>
-    <t>151s (uh)</t>
-  </si>
-  <si>
-    <t>97s (uh)</t>
-  </si>
-  <si>
-    <t>82s (uh)</t>
-  </si>
-  <si>
-    <t>855s (uh)</t>
-  </si>
-  <si>
     <t>28444,1…</t>
   </si>
   <si>
-    <t>2328s (uh)</t>
-  </si>
-  <si>
     <t>time_limit=1200, never exceeded</t>
   </si>
   <si>
     <t>55302,6…</t>
   </si>
   <si>
-    <t>2154s (uh)</t>
-  </si>
-  <si>
     <t>12939,6…</t>
   </si>
   <si>
-    <t>8000s (uh)</t>
-  </si>
-  <si>
     <t>371,2…</t>
   </si>
   <si>
     <t>5s</t>
+  </si>
+  <si>
+    <t>68164,1…</t>
+  </si>
+  <si>
+    <t>464,2…</t>
+  </si>
+  <si>
+    <t>512,6…</t>
+  </si>
+  <si>
+    <t>12s</t>
+  </si>
+  <si>
+    <t>1s</t>
+  </si>
+  <si>
+    <t>13s</t>
+  </si>
+  <si>
+    <t>32s</t>
+  </si>
+  <si>
+    <t>3s</t>
+  </si>
+  <si>
+    <t>60s</t>
+  </si>
+  <si>
+    <t>16s</t>
+  </si>
+  <si>
+    <t>855s</t>
+  </si>
+  <si>
+    <t>151s</t>
+  </si>
+  <si>
+    <t>97s</t>
+  </si>
+  <si>
+    <t>82s</t>
+  </si>
+  <si>
+    <t>282s</t>
+  </si>
+  <si>
+    <t>48s</t>
+  </si>
+  <si>
+    <t>114s</t>
+  </si>
+  <si>
+    <t>246s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">80s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">210s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8000s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2154s </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2328s </t>
+  </si>
+  <si>
+    <t>1042,2…</t>
+  </si>
+  <si>
+    <t>27080,0…</t>
+  </si>
+  <si>
+    <t>27250,…</t>
+  </si>
+  <si>
+    <t>25409,9..</t>
+  </si>
+  <si>
+    <t>14510,8…</t>
+  </si>
+  <si>
+    <t>4700s old</t>
+  </si>
+  <si>
+    <t>14s</t>
+  </si>
+  <si>
+    <t>31s</t>
+  </si>
+  <si>
+    <t>18s</t>
+  </si>
+  <si>
+    <t>5.39516843971631e+02… (aktuelle Lösung ist drüber!)</t>
   </si>
 </sst>
 </file>
@@ -437,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -446,6 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -763,7 +773,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,7 +783,7 @@
     <col min="4" max="4" width="10.83203125" style="4"/>
     <col min="5" max="5" width="36.5" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="4"/>
     <col min="9" max="9" width="10.83203125" style="5"/>
     <col min="10" max="10" width="24.1640625" style="7" bestFit="1" customWidth="1"/>
@@ -793,9 +803,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>69</v>
-      </c>
+      <c r="E1" s="6"/>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
@@ -804,16 +812,16 @@
         <v>5</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1">
         <v>8</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="O1" s="1">
         <v>20</v>
@@ -821,7 +829,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>375</v>
@@ -832,23 +840,26 @@
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="E2" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="F2" s="4" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="L2">
         <v>373.5</v>
       </c>
       <c r="M2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O2" t="s">
         <v>7</v>
@@ -856,7 +867,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>569</v>
@@ -867,28 +878,34 @@
       <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
+      <c r="E3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>88</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="N3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>534</v>
@@ -897,33 +914,33 @@
         <v>47</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>12</v>
+      <c r="F4" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="M4" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="N4" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>835</v>
@@ -932,27 +949,27 @@
         <v>136</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="L5" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>521</v>
@@ -961,60 +978,60 @@
         <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>76</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="H6" s="7"/>
       <c r="L6" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>1021</v>
       </c>
       <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="H7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" t="s">
         <v>27</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" t="s">
-        <v>83</v>
-      </c>
-      <c r="N7" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>1067</v>
@@ -1023,18 +1040,21 @@
         <v>114</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>71</v>
+        <v>79</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="L8" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>27591</v>
@@ -1043,21 +1063,24 @@
         <v>140</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>74</v>
+        <v>11</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="L10" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="M10" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>26362</v>
@@ -1066,18 +1089,21 @@
         <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="L11" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>14971</v>
@@ -1086,21 +1112,24 @@
         <v>16</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="L12" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="M12" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B13">
         <v>12747</v>
@@ -1109,15 +1138,15 @@
         <v>171</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>13332</v>
@@ -1126,24 +1155,24 @@
         <v>23</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="L14" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="M14" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="N14" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>55539</v>
@@ -1152,24 +1181,24 @@
         <v>128</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="L15" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="M15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N15" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>28940</v>
@@ -1178,24 +1207,24 @@
         <v>41</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="L16" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="M16" t="s">
         <v>96</v>
       </c>
       <c r="N16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B17">
         <v>58578</v>
@@ -1204,12 +1233,12 @@
         <v>83</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>25742</v>
@@ -1218,9 +1247,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B19">
         <v>38684</v>
@@ -1229,23 +1258,23 @@
         <v>16</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C20">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>95151</v>
@@ -1254,24 +1283,27 @@
         <v>269</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>15</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E22" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>67</v>
+      <c r="G22" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new espprc results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51CB3A0-C603-4E4C-AF9F-8907E2F1E9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8634ABD-619A-2B42-B7F6-7F1736D368E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="109">
   <si>
     <t>Instanz</t>
   </si>
@@ -232,9 +232,6 @@
     <t>14704,8…</t>
   </si>
   <si>
-    <t xml:space="preserve">time_limit 600 exceeded </t>
-  </si>
-  <si>
     <t>(uh) time_limit 1200 exceeded (gesamt 3800s)</t>
   </si>
   <si>
@@ -356,6 +353,15 @@
   </si>
   <si>
     <t>5.39516843971631e+02… (aktuelle Lösung ist drüber!)</t>
+  </si>
+  <si>
+    <t>484,7…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4430s </t>
+  </si>
+  <si>
+    <t>cspy</t>
   </si>
 </sst>
 </file>
@@ -446,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -456,6 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -772,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -841,25 +848,25 @@
         <v>6</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L2">
         <v>373.5</v>
       </c>
       <c r="M2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O2" t="s">
         <v>7</v>
@@ -879,25 +886,25 @@
         <v>8</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>35</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N3" t="s">
         <v>59</v>
@@ -920,19 +927,25 @@
         <v>11</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>65</v>
+        <v>106</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>108</v>
       </c>
       <c r="L4" t="s">
         <v>24</v>
       </c>
       <c r="M4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N4" t="s">
         <v>62</v>
@@ -958,7 +971,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>37</v>
@@ -981,13 +994,13 @@
         <v>17</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6" s="7"/>
       <c r="L6" t="s">
@@ -1008,13 +1021,13 @@
         <v>19</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>37</v>
@@ -1023,7 +1036,7 @@
         <v>25</v>
       </c>
       <c r="M7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N7" t="s">
         <v>27</v>
@@ -1043,10 +1056,10 @@
         <v>29</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L8" t="s">
         <v>61</v>
@@ -1069,13 +1082,13 @@
         <v>11</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" t="s">
         <v>98</v>
       </c>
-      <c r="L10" t="s">
-        <v>99</v>
-      </c>
       <c r="M10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -1092,13 +1105,13 @@
         <v>46</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -1115,16 +1128,16 @@
         <v>39</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L12" t="s">
         <v>64</v>
       </c>
       <c r="M12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1141,7 +1154,7 @@
         <v>44</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1158,16 +1171,16 @@
         <v>45</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -1184,16 +1197,16 @@
         <v>47</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -1210,16 +1223,16 @@
         <v>48</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L16" t="s">
+        <v>66</v>
+      </c>
+      <c r="M16" t="s">
+        <v>95</v>
+      </c>
+      <c r="N16" t="s">
         <v>67</v>
-      </c>
-      <c r="M16" t="s">
-        <v>96</v>
-      </c>
-      <c r="N16" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1297,13 +1310,13 @@
         <v>57</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use heuristic for finding multiple routes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFE60F0-B561-BF44-A7A0-0E04FD481541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92574CB6-3076-AB47-AA30-54230D8F6415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="113">
   <si>
     <t>Instanz</t>
   </si>
@@ -280,9 +280,6 @@
     <t>16s</t>
   </si>
   <si>
-    <t>855s</t>
-  </si>
-  <si>
     <t>151s</t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     <t xml:space="preserve">90s </t>
   </si>
   <si>
-    <t xml:space="preserve">80s </t>
-  </si>
-  <si>
     <t xml:space="preserve">210s </t>
   </si>
   <si>
@@ -362,6 +356,24 @@
   </si>
   <si>
     <t>20s</t>
+  </si>
+  <si>
+    <t>6s (ht=0.1,hit=100)</t>
+  </si>
+  <si>
+    <t>120s, hit=1e4, ht=1e-3</t>
+  </si>
+  <si>
+    <t>210s, hit=1e4, ht=1e-3</t>
+  </si>
+  <si>
+    <t>12519,1…</t>
+  </si>
+  <si>
+    <t>time_limit=300, never exceeded</t>
+  </si>
+  <si>
+    <t>time_limit=36e3 exceeded ohne Heuristik</t>
   </si>
 </sst>
 </file>
@@ -779,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -889,22 +901,25 @@
         <v>76</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>34</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="L3" t="s">
         <v>22</v>
       </c>
       <c r="M3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N3" t="s">
         <v>58</v>
@@ -930,22 +945,22 @@
         <v>72</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
       </c>
       <c r="M4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N4" t="s">
         <v>61</v>
@@ -965,7 +980,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>14</v>
@@ -1000,7 +1015,7 @@
         <v>73</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H6" s="7"/>
       <c r="L6" t="s">
@@ -1036,7 +1051,7 @@
         <v>24</v>
       </c>
       <c r="M7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N7" t="s">
         <v>26</v>
@@ -1059,7 +1074,7 @@
         <v>77</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L8" t="s">
         <v>60</v>
@@ -1082,13 +1097,13 @@
         <v>11</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M10" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -1108,7 +1123,7 @@
         <v>79</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L11" t="s">
         <v>64</v>
@@ -1131,13 +1146,13 @@
         <v>80</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L12" t="s">
         <v>63</v>
       </c>
       <c r="M12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -1154,7 +1169,16 @@
         <v>43</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>81</v>
+        <v>108</v>
+      </c>
+      <c r="L13" t="s">
+        <v>110</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="N13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1171,13 +1195,13 @@
         <v>44</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L14" t="s">
         <v>68</v>
       </c>
       <c r="M14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="N14" t="s">
         <v>66</v>
@@ -1197,13 +1221,13 @@
         <v>46</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L15" t="s">
         <v>67</v>
       </c>
       <c r="M15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N15" t="s">
         <v>66</v>
@@ -1223,13 +1247,13 @@
         <v>47</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L16" t="s">
         <v>65</v>
       </c>
       <c r="M16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N16" t="s">
         <v>66</v>
@@ -1310,13 +1334,13 @@
         <v>56</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>71</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add load check for new paths
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2B4008-8CD7-EA45-A634-30D6758ED724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5AE009-525A-5043-B0A9-F73DCB00CE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45880" yWindow="0" windowWidth="22920" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="117">
   <si>
     <t>Instanz</t>
   </si>
@@ -229,9 +229,6 @@
     <t>14704,8…</t>
   </si>
   <si>
-    <t>(uh) time_limit 1200 exceeded (gesamt 3800s)</t>
-  </si>
-  <si>
     <t>28444,1…</t>
   </si>
   <si>
@@ -340,15 +337,6 @@
     <t>5.39516843971631e+02… (aktuelle Lösung ist drüber!)</t>
   </si>
   <si>
-    <t>484,7…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4430s </t>
-  </si>
-  <si>
-    <t>cspy (ab dem Zeitpunkt wo Labelling scheitert ausschließlich)</t>
-  </si>
-  <si>
     <t>20s</t>
   </si>
   <si>
@@ -377,6 +365,27 @@
   </si>
   <si>
     <t>29s ,hit=2e3, ht=0.1, hst=20</t>
+  </si>
+  <si>
+    <t>time_limit=36e2 exceeded, 200 initial variables</t>
+  </si>
+  <si>
+    <t>time_limit=36e2 exceeded, 15306 initial variables</t>
+  </si>
+  <si>
+    <t>time_limit=36e2 exceeded, 6788 initial variables</t>
+  </si>
+  <si>
+    <t>time_limit 3600 exceeded, 6790 initial variables</t>
+  </si>
+  <si>
+    <t>time_limit=3600 exceeded, 12957 initial variables</t>
+  </si>
+  <si>
+    <t>X-n172-k51</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -792,27 +801,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="4"/>
-    <col min="5" max="5" width="36.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="4"/>
-    <col min="9" max="9" width="10.83203125" style="5"/>
-    <col min="10" max="10" width="24.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="4"/>
+    <col min="6" max="6" width="36.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="4"/>
+    <col min="10" max="10" width="10.83203125" style="5"/>
+    <col min="11" max="11" width="24.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -820,533 +830,549 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="1">
+      <c r="M1" s="1">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P1" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B2">
         <v>375</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>32</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="F2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="L2">
+      <c r="J2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2">
         <v>373.5</v>
       </c>
-      <c r="M2" t="s">
-        <v>75</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B3">
         <v>569</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>69</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="F3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="L3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" t="s">
-        <v>85</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
         <v>534</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>47</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>98</v>
+      <c r="G4" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="L4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="M4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" t="s">
-        <v>86</v>
-      </c>
       <c r="N4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
         <v>835</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>136</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="H5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6">
         <v>521</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>42</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="L6" t="s">
+      <c r="G6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="M6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7">
         <v>1021</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="M7" t="s">
         <v>24</v>
       </c>
-      <c r="M7" t="s">
-        <v>87</v>
-      </c>
       <c r="N7" t="s">
+        <v>86</v>
+      </c>
+      <c r="O7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8">
         <v>1067</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>114</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="F8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
       <c r="B10">
         <v>27591</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>140</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="M10" t="s">
         <v>92</v>
       </c>
-      <c r="L10" t="s">
-        <v>93</v>
-      </c>
-      <c r="M10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
       <c r="B11">
         <v>26362</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>14</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="M11" t="s">
         <v>113</v>
       </c>
-      <c r="L11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>37</v>
       </c>
       <c r="B12">
         <v>14971</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>16</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="F12" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M12" t="s">
         <v>63</v>
       </c>
-      <c r="M12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>39</v>
       </c>
       <c r="B13">
         <v>12747</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>171</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="L13" t="s">
-        <v>108</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="N13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F13" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="M13" t="s">
+        <v>104</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="O13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
       <c r="B14">
         <v>13332</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>23</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="L14" t="s">
-        <v>68</v>
+      <c r="F14" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="M14" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="N14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="O14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>41</v>
       </c>
       <c r="B15">
         <v>55539</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>128</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="L15" t="s">
-        <v>67</v>
+      <c r="F15" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="M15" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="N15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="O15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16">
         <v>28940</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>41</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M16" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" t="s">
+        <v>89</v>
+      </c>
+      <c r="O16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17">
+        <v>45607</v>
+      </c>
+      <c r="C17">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18">
+        <v>58578</v>
+      </c>
+      <c r="D18">
+        <v>83</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19">
+        <v>25742</v>
+      </c>
+      <c r="D19">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20">
+        <v>38684</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22">
+        <v>95151</v>
+      </c>
+      <c r="D22">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="L16" t="s">
-        <v>65</v>
-      </c>
-      <c r="M16" t="s">
-        <v>90</v>
-      </c>
-      <c r="N16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17">
-        <v>58578</v>
-      </c>
-      <c r="C17">
-        <v>83</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18">
-        <v>25742</v>
-      </c>
-      <c r="C18">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19">
-        <v>38684</v>
-      </c>
-      <c r="C19">
-        <v>16</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21">
-        <v>95151</v>
-      </c>
-      <c r="C21">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22">
-        <v>15</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>96</v>
+      <c r="G23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Write initial heuristic params to output
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5A2DFA-4F37-C44C-8E5F-53A83D6BC021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A229A69B-2D5E-0341-88C8-366D78218BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45880" yWindow="0" windowWidth="22920" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add new results for ng
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A229A69B-2D5E-0341-88C8-366D78218BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4500FBE1-BB62-FB45-8974-B61468CA76D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45880" yWindow="0" windowWidth="22920" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="21000" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="126">
   <si>
     <t>Instanz</t>
   </si>
@@ -106,18 +106,9 @@
     <t>558,6…</t>
   </si>
   <si>
-    <t>481,0…</t>
-  </si>
-  <si>
-    <t>1002,2…</t>
-  </si>
-  <si>
     <t>Beobachtung</t>
   </si>
   <si>
-    <t>Nur eine verwendete Variable ist nicht elementar. DSSR sinnvoll für ESPPRC Lösung?</t>
-  </si>
-  <si>
     <t>E-n101-k14</t>
   </si>
   <si>
@@ -211,33 +202,9 @@
     <t>X-n502-k39</t>
   </si>
   <si>
-    <t>time_limit=10</t>
-  </si>
-  <si>
     <t>52 (realistisch 7)</t>
   </si>
   <si>
-    <t>(uh) time_limit 300 exceeded</t>
-  </si>
-  <si>
-    <t>time_limi=30</t>
-  </si>
-  <si>
-    <t>time_limit=60 exceeded</t>
-  </si>
-  <si>
-    <t>14704,8…</t>
-  </si>
-  <si>
-    <t>28444,1…</t>
-  </si>
-  <si>
-    <t>time_limit=1200, never exceeded</t>
-  </si>
-  <si>
-    <t>55302,6…</t>
-  </si>
-  <si>
     <t>12939,6…</t>
   </si>
   <si>
@@ -289,33 +256,12 @@
     <t>48s</t>
   </si>
   <si>
-    <t>114s</t>
-  </si>
-  <si>
-    <t>246s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90s </t>
-  </si>
-  <si>
-    <t xml:space="preserve">210s </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2154s </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2328s </t>
-  </si>
-  <si>
     <t>1042,2…</t>
   </si>
   <si>
     <t>27080,0…</t>
   </si>
   <si>
-    <t>27250,…</t>
-  </si>
-  <si>
     <t>25409,9..</t>
   </si>
   <si>
@@ -340,24 +286,9 @@
     <t>20s</t>
   </si>
   <si>
-    <t>6s (ht=0.1,hit=100)</t>
-  </si>
-  <si>
     <t>120s, hit=1e4, ht=1e-3</t>
   </si>
   <si>
-    <t>210s, hit=1e4, ht=1e-3</t>
-  </si>
-  <si>
-    <t>12519,1…</t>
-  </si>
-  <si>
-    <t>time_limit=300, never exceeded</t>
-  </si>
-  <si>
-    <t>900s, hit=1e4, ht=1e-3</t>
-  </si>
-  <si>
     <t>time_limit=36e2 never exceeded</t>
   </si>
   <si>
@@ -427,7 +358,61 @@
     <t>24000s</t>
   </si>
   <si>
-    <t>5600s</t>
+    <t>4s</t>
+  </si>
+  <si>
+    <t>25s</t>
+  </si>
+  <si>
+    <t>480,5…</t>
+  </si>
+  <si>
+    <t>802,9..</t>
+  </si>
+  <si>
+    <t>517,0…</t>
+  </si>
+  <si>
+    <t>7s</t>
+  </si>
+  <si>
+    <t>1001,8…</t>
+  </si>
+  <si>
+    <t>27254,1…</t>
+  </si>
+  <si>
+    <t>19s</t>
+  </si>
+  <si>
+    <t>27244,6…</t>
+  </si>
+  <si>
+    <t>14701,2…</t>
+  </si>
+  <si>
+    <t>28439,0…</t>
+  </si>
+  <si>
+    <t>36s</t>
+  </si>
+  <si>
+    <t>12507,8…</t>
+  </si>
+  <si>
+    <t>325s</t>
+  </si>
+  <si>
+    <t>55297,3…</t>
+  </si>
+  <si>
+    <t>1044,8…</t>
+  </si>
+  <si>
+    <t>193s</t>
+  </si>
+  <si>
+    <t>Sehr hohe Anzahl an Iterationen! Gut für die Bachelorarbeit?</t>
   </si>
 </sst>
 </file>
@@ -526,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -538,6 +523,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -854,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -898,7 +885,7 @@
         <v>5</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>20</v>
@@ -907,7 +894,7 @@
         <v>8</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P1" s="1">
         <v>20</v>
@@ -915,7 +902,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>375</v>
@@ -927,28 +914,31 @@
         <v>6</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="M2">
         <v>373.5</v>
       </c>
       <c r="N2" t="s">
-        <v>74</v>
-      </c>
-      <c r="P2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="11" t="s">
         <v>7</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -965,31 +955,34 @@
         <v>8</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="M3" t="s">
         <v>22</v>
       </c>
       <c r="N3" t="s">
-        <v>84</v>
-      </c>
-      <c r="O3" t="s">
-        <v>58</v>
+        <v>107</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1009,29 +1002,28 @@
         <v>11</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="N4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O4" t="s">
-        <v>61</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1047,20 +1039,25 @@
         <v>13</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M5" t="s">
-        <v>62</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="N5" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1076,18 +1073,23 @@
         <v>16</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="I6" s="7"/>
       <c r="M6" t="s">
-        <v>62</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="N6" t="s">
+        <v>112</v>
+      </c>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1097,48 +1099,45 @@
         <v>1021</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="M7" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="N7" t="s">
-        <v>86</v>
-      </c>
-      <c r="O7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>130</v>
+        <v>63</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>1067</v>
@@ -1147,21 +1146,24 @@
         <v>114</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="M8" t="s">
-        <v>60</v>
+        <v>123</v>
+      </c>
+      <c r="N8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>27591</v>
@@ -1173,27 +1175,34 @@
         <v>140</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="M10" t="s">
-        <v>92</v>
-      </c>
-      <c r="N10" t="s">
-        <v>101</v>
+        <v>87</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>26362</v>
@@ -1205,27 +1214,31 @@
         <v>14</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="M11" t="s">
-        <v>112</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>14971</v>
@@ -1237,30 +1250,33 @@
         <v>16</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="M12" t="s">
-        <v>63</v>
-      </c>
-      <c r="N12" t="s">
-        <v>87</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13">
         <v>12747</v>
@@ -1272,30 +1288,30 @@
         <v>171</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="M13" t="s">
-        <v>104</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="O13" t="s">
-        <v>105</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>13332</v>
@@ -1307,36 +1323,38 @@
         <v>23</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="N14" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="M14" t="s">
-        <v>67</v>
-      </c>
-      <c r="N14" t="s">
-        <v>106</v>
-      </c>
-      <c r="O14" t="s">
-        <v>105</v>
-      </c>
+      <c r="O14" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>55539</v>
@@ -1348,30 +1366,30 @@
         <v>128</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="I15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M15" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="K15" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="M15" t="s">
-        <v>66</v>
-      </c>
-      <c r="N15" t="s">
-        <v>88</v>
-      </c>
-      <c r="O15" t="s">
-        <v>65</v>
-      </c>
+      <c r="N15" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <v>28940</v>
@@ -1383,25 +1401,25 @@
         <v>41</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="I16" s="10"/>
-      <c r="M16" t="s">
-        <v>64</v>
-      </c>
-      <c r="N16" t="s">
-        <v>89</v>
-      </c>
-      <c r="O16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M16" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="B17">
         <v>45607</v>
@@ -1412,10 +1430,13 @@
       <c r="D17">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>58578</v>
@@ -1427,12 +1448,15 @@
         <v>83</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19">
         <v>25742</v>
@@ -1444,9 +1468,9 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B20">
         <v>38684</v>
@@ -1458,15 +1482,15 @@
         <v>16</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>55</v>
       </c>
       <c r="C21">
         <v>16</v>
@@ -1475,9 +1499,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B22">
         <v>95151</v>
@@ -1489,12 +1513,12 @@
         <v>269</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C23">
         <v>39</v>
@@ -1503,16 +1527,16 @@
         <v>15</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add total scip time to the output log
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224A629D-BEF5-F349-A1E7-A4A6B837D6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1417FC30-8C3E-E74E-85E3-C7DD077BF5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34400" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="135">
   <si>
     <t>Instanz</t>
   </si>
@@ -422,6 +422,24 @@
   </si>
   <si>
     <t>1442s</t>
+  </si>
+  <si>
+    <t>3300s</t>
+  </si>
+  <si>
+    <t>803,3..</t>
+  </si>
+  <si>
+    <t>1 non elementary path</t>
+  </si>
+  <si>
+    <t>2020s</t>
+  </si>
+  <si>
+    <t>14735,9…</t>
+  </si>
+  <si>
+    <t>elementary, sehr ungleiche Laufzeit</t>
   </si>
 </sst>
 </file>
@@ -855,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -876,7 +894,7 @@
     <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -916,7 +934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -957,7 +975,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -998,7 +1016,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1035,10 +1053,17 @@
       <c r="N4" t="s">
         <v>61</v>
       </c>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P4" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1075,10 +1100,17 @@
       <c r="N5" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P5" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1114,7 +1146,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>115</v>
       </c>
@@ -1130,7 +1162,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>116</v>
       </c>
@@ -1149,7 +1181,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -1165,7 +1197,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1209,7 +1241,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -1222,7 +1254,7 @@
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1263,7 +1295,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1302,7 +1334,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1346,7 +1378,7 @@
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1384,8 +1416,15 @@
         <v>63</v>
       </c>
       <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
+      <c r="P16" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Add script to multitask code
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1417FC30-8C3E-E74E-85E3-C7DD077BF5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B4CA13-4F34-A646-A8D3-32657AE86E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34400" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
+    <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -876,7 +876,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add time measurements to output file
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B4CA13-4F34-A646-A8D3-32657AE86E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E997A670-9913-9E4C-A169-0F4A0A0617D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
+    <workbookView xWindow="34400" yWindow="0" windowWidth="34400" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="146">
   <si>
     <t>Instanz</t>
   </si>
@@ -440,6 +440,39 @@
   </si>
   <si>
     <t>elementary, sehr ungleiche Laufzeit</t>
+  </si>
+  <si>
+    <t>55313,4…</t>
+  </si>
+  <si>
+    <t>22000s</t>
+  </si>
+  <si>
+    <t>half non elementary</t>
+  </si>
+  <si>
+    <t>28501,73…</t>
+  </si>
+  <si>
+    <t>5200s</t>
+  </si>
+  <si>
+    <t>12568.6…</t>
+  </si>
+  <si>
+    <t>4600s</t>
+  </si>
+  <si>
+    <t>787.0…</t>
+  </si>
+  <si>
+    <t>7300s</t>
+  </si>
+  <si>
+    <t>45271.2…</t>
+  </si>
+  <si>
+    <t>14000s</t>
   </si>
 </sst>
 </file>
@@ -876,7 +909,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E31" activeCellId="1" sqref="I10 E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1189,7 +1222,15 @@
         <v>830</v>
       </c>
       <c r="G9" s="8"/>
-      <c r="J9" s="9"/>
+      <c r="I9" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>113</v>
+      </c>
       <c r="P9" s="12" t="s">
         <v>123</v>
       </c>
@@ -1249,10 +1290,21 @@
         <v>817</v>
       </c>
       <c r="G11" s="8"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="9"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
+      <c r="I11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="P11" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1317,6 +1369,12 @@
       <c r="G14" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="I14" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>114</v>
+      </c>
       <c r="K14" s="7" t="s">
         <v>113</v>
       </c>
@@ -1426,7 +1484,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1461,10 +1519,14 @@
         <v>106</v>
       </c>
       <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P17" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q17" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1507,7 +1569,7 @@
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1542,10 +1604,17 @@
         <v>67</v>
       </c>
       <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P19" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="R19" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1580,10 +1649,17 @@
         <v>104</v>
       </c>
       <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="12"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P20" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q20" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="R20" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -1608,8 +1684,14 @@
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P21" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q21" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1638,7 +1720,7 @@
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1661,7 +1743,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1687,7 +1769,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1710,7 +1792,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1733,7 +1815,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Fix a bug in the output
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0805D6A5-D769-7049-A60A-3BBAD520877A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF612BB-6AE0-844F-A38B-C3CA736ACB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="0" windowWidth="34400" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
+    <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -919,7 +919,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E31" activeCellId="1" sqref="I10 E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update run.py for uchoa run
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF612BB-6AE0-844F-A38B-C3CA736ACB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AB43C2-3E1F-CD40-A86D-2C2CB5F832AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="161">
   <si>
     <t>Instanz</t>
   </si>
@@ -482,6 +482,42 @@
   </si>
   <si>
     <t>200000s</t>
+  </si>
+  <si>
+    <t>X-n148-k46</t>
+  </si>
+  <si>
+    <t>X-n153-k22</t>
+  </si>
+  <si>
+    <t>X-n195-k51</t>
+  </si>
+  <si>
+    <t>X-n233-k16</t>
+  </si>
+  <si>
+    <t>X-n247-k50</t>
+  </si>
+  <si>
+    <t>X-n270-k35</t>
+  </si>
+  <si>
+    <t>X-n294-k50</t>
+  </si>
+  <si>
+    <t>X-n313-k71</t>
+  </si>
+  <si>
+    <t>X-n384-k52</t>
+  </si>
+  <si>
+    <t>X-n336-k84</t>
+  </si>
+  <si>
+    <t>X-n429-k61</t>
+  </si>
+  <si>
+    <t>X-n469-k138</t>
   </si>
 </sst>
 </file>
@@ -916,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B037F8AC-8353-4449-B388-5B9B0D49B938}">
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" activeCellId="1" sqref="I10 E31"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1685,77 +1721,48 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21">
-        <v>45607</v>
+        <v>149</v>
       </c>
       <c r="C21" s="11">
-        <v>53</v>
-      </c>
-      <c r="D21">
-        <v>83</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>111</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="I21" s="10"/>
+      <c r="J21" s="9"/>
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
-      <c r="P21" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q21" s="9" t="s">
-        <v>143</v>
-      </c>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22">
-        <v>58578</v>
-      </c>
-      <c r="C22">
-        <v>36</v>
-      </c>
-      <c r="D22">
-        <v>83</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>111</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="C22" s="11">
+        <v>23</v>
+      </c>
+      <c r="I22" s="10"/>
+      <c r="J22" s="9"/>
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="B23">
-        <v>25742</v>
-      </c>
-      <c r="C23">
-        <v>23</v>
+        <v>45607</v>
+      </c>
+      <c r="C23" s="11">
+        <v>53</v>
       </c>
       <c r="D23">
-        <v>156</v>
+        <v>83</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>112</v>
@@ -1766,45 +1773,44 @@
       <c r="K23" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24">
-        <v>38684</v>
-      </c>
-      <c r="C24">
-        <v>28</v>
-      </c>
-      <c r="D24">
-        <v>16</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>111</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="C24" s="11">
+        <v>53</v>
+      </c>
+      <c r="J24" s="9"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>58578</v>
       </c>
       <c r="C25">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D25">
-        <v>27</v>
+        <v>83</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>112</v>
@@ -1815,62 +1821,221 @@
       <c r="K25" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26">
-        <v>95151</v>
+        <v>152</v>
       </c>
       <c r="C26" s="11">
-        <v>61</v>
-      </c>
-      <c r="D26">
-        <v>269</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>111</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27">
+        <v>25742</v>
+      </c>
+      <c r="C27">
+        <v>23</v>
+      </c>
+      <c r="D27">
+        <v>156</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28">
+        <v>38684</v>
+      </c>
+      <c r="C28">
+        <v>28</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29">
+        <v>51</v>
+      </c>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30">
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <v>27</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" s="11">
+        <v>36</v>
+      </c>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32">
+        <v>95151</v>
+      </c>
+      <c r="C32" s="11">
+        <v>61</v>
+      </c>
+      <c r="D32">
+        <v>269</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="11">
+        <v>51</v>
+      </c>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="11">
+        <v>72</v>
+      </c>
+      <c r="J34" s="9"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>158</v>
+      </c>
+      <c r="C35" s="11">
+        <v>86</v>
+      </c>
+      <c r="J35" s="9"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36" s="11">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
+      <c r="J36" s="9"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="11">
+        <v>62</v>
+      </c>
+      <c r="J37" s="9"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="11">
+        <v>139</v>
+      </c>
+      <c r="J38" s="9"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" t="s">
         <v>50</v>
       </c>
-      <c r="C27">
+      <c r="C39">
         <v>39</v>
       </c>
-      <c r="D27">
+      <c r="D39">
         <v>15</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H39" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="K27" s="7" t="s">
+      <c r="I39" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="K39" s="7" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ESPPRC heuristic version
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/habanzu/Dropbox/Bachelorarbeit/cvrp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AB43C2-3E1F-CD40-A86D-2C2CB5F832AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75DBFB1-5B54-DA42-A839-0A0F159DBCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22920" yWindow="0" windowWidth="22940" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
+    <workbookView xWindow="22940" yWindow="0" windowWidth="45860" windowHeight="28800" xr2:uid="{86ED8C44-9F2A-2D49-988F-F887C17EEBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="162">
   <si>
     <t>Instanz</t>
   </si>
@@ -310,9 +310,6 @@
     <t>484,0…</t>
   </si>
   <si>
-    <t>24000s</t>
-  </si>
-  <si>
     <t>4s</t>
   </si>
   <si>
@@ -388,9 +385,6 @@
     <t>E-n101-k8</t>
   </si>
   <si>
-    <t>200s</t>
-  </si>
-  <si>
     <t>20000s</t>
   </si>
   <si>
@@ -518,6 +512,15 @@
   </si>
   <si>
     <t>X-n469-k138</t>
+  </si>
+  <si>
+    <t>ESPPRC_heur</t>
+  </si>
+  <si>
+    <t>61s</t>
+  </si>
+  <si>
+    <t>elementary, ESPPRC_heur</t>
   </si>
 </sst>
 </file>
@@ -955,7 +958,7 @@
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1086,13 +1089,13 @@
         <v>22</v>
       </c>
       <c r="N3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P3" s="12" t="s">
         <v>31</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -1121,13 +1124,13 @@
         <v>90</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="M4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N4" t="s">
         <v>61</v>
@@ -1136,10 +1139,10 @@
         <v>90</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -1165,28 +1168,28 @@
         <v>64</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N5" t="s">
         <v>77</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q5" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="R5" s="12" t="s">
         <v>127</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1213,21 +1216,24 @@
       </c>
       <c r="J6" s="9"/>
       <c r="M6" t="s">
+        <v>95</v>
+      </c>
+      <c r="N6" t="s">
         <v>96</v>
       </c>
-      <c r="N6" t="s">
-        <v>97</v>
-      </c>
       <c r="P6" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>117</v>
+        <v>160</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7">
         <v>682</v>
@@ -1235,15 +1241,15 @@
       <c r="G7" s="8"/>
       <c r="J7" s="9"/>
       <c r="P7" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8">
         <v>735</v>
@@ -1254,34 +1260,34 @@
       <c r="G8" s="8"/>
       <c r="J8" s="9"/>
       <c r="P8" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9">
         <v>830</v>
       </c>
       <c r="G9" s="8"/>
       <c r="I9" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1310,13 +1316,13 @@
         <v>89</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N10" t="s">
         <v>62</v>
@@ -1330,26 +1336,26 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11">
         <v>817</v>
       </c>
       <c r="G11" s="8"/>
       <c r="I11" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1372,25 +1378,25 @@
         <v>72</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N12" t="s">
         <v>57</v>
       </c>
       <c r="P12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -1416,23 +1422,23 @@
         <v>73</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>62</v>
       </c>
       <c r="O14" s="12"/>
       <c r="P14" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q14" s="9" t="s">
         <v>63</v>
@@ -1464,26 +1470,26 @@
         <v>84</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N15" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -1509,29 +1515,29 @@
         <v>75</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N16" s="12" t="s">
         <v>63</v>
       </c>
       <c r="O16" s="12"/>
       <c r="P16" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="R16" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -1554,26 +1560,26 @@
         <v>82</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M17" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="N17" s="13" t="s">
         <v>104</v>
-      </c>
-      <c r="N17" s="13" t="s">
-        <v>105</v>
       </c>
       <c r="O17" s="12"/>
       <c r="P17" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -1602,31 +1608,31 @@
         <v>87</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M18" s="12" t="s">
         <v>55</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="R18" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -1649,29 +1655,29 @@
         <v>68</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N19" s="12" t="s">
         <v>67</v>
       </c>
       <c r="O19" s="12"/>
       <c r="P19" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="R19" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="Q19" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="R19" s="9" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -1694,34 +1700,34 @@
         <v>69</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M20" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="N20" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="N20" s="12" t="s">
-        <v>103</v>
       </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C21" s="11">
         <v>47</v>
@@ -1737,7 +1743,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C22" s="11">
         <v>23</v>
@@ -1765,27 +1771,27 @@
         <v>83</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
       <c r="P23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q23" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C24" s="11">
         <v>53</v>
@@ -1813,13 +1819,13 @@
         <v>46</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M25" s="12"/>
       <c r="N25" s="12"/>
@@ -1827,7 +1833,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C26" s="11">
         <v>17</v>
@@ -1851,13 +1857,13 @@
         <v>156</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -1877,18 +1883,18 @@
         <v>48</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C29">
         <v>51</v>
@@ -1909,18 +1915,18 @@
         <v>27</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C31" s="11">
         <v>36</v>
@@ -1941,18 +1947,18 @@
         <v>269</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C33" s="11">
         <v>51</v>
@@ -1961,7 +1967,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C34" s="11">
         <v>72</v>
@@ -1970,7 +1976,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C35" s="11">
         <v>86</v>
@@ -1979,7 +1985,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C36" s="11">
         <v>53</v>
@@ -1988,7 +1994,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C37" s="11">
         <v>62</v>
@@ -1997,7 +2003,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C38" s="11">
         <v>139</v>
@@ -2030,13 +2036,13 @@
         <v>76</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>